<commit_message>
Final Design: High voltage logos were added High voltage clearance checked * were added to boot pins 100A & 4A (optional ) CTs  were added to BOM ERC & DRC were made
</commit_message>
<xml_diff>
--- a/H2AR30/Release/BOM/H2AR30.xlsx
+++ b/H2AR30/Release/BOM/H2AR30.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="142">
   <si>
     <t>Qty</t>
   </si>
@@ -415,13 +415,43 @@
   </si>
   <si>
     <t xml:space="preserve">BI-zener 3.3v </t>
+  </si>
+  <si>
+    <t>100 A current Transformer</t>
+  </si>
+  <si>
+    <t>CR Magnetics</t>
+  </si>
+  <si>
+    <t>CR8450-1000</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cr8450-1000-cr+magnetics-19500880?r=sp</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>CR8401-1000-G</t>
+  </si>
+  <si>
+    <t>4 A current Transformer</t>
+  </si>
+  <si>
+    <t>Curr Sense Xfmr 100A In-line 1000:1</t>
+  </si>
+  <si>
+    <t>Curr Sense Xfmr 4A In-line 1000:1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cr8401-1000-g-cr+magnetics-1366028?r=sp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,6 +586,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -854,7 +892,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -897,8 +935,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -906,8 +945,11 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -941,6 +983,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1227,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1742,7 @@
       <c r="F20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1722,7 +1765,7 @@
       <c r="F21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1908,12 +1951,61 @@
       </c>
       <c r="G29" s="1" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:G31">
     <sortCondition ref="C1"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="G30" r:id="rId1"/>
+    <hyperlink ref="G20" r:id="rId2"/>
+    <hyperlink ref="G21" r:id="rId3"/>
+    <hyperlink ref="G31" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final with double check
</commit_message>
<xml_diff>
--- a/H2AR30/Release/BOM/H2AR30.xlsx
+++ b/H2AR30/Release/BOM/H2AR30.xlsx
@@ -198,9 +198,6 @@
     <t>1M0</t>
   </si>
   <si>
-    <t>R8, R9, R10</t>
-  </si>
-  <si>
     <t>RT1206BRD071ML</t>
   </si>
   <si>
@@ -445,6 +442,9 @@
   </si>
   <si>
     <t>https://octopart.com/cr8401-1000-g-cr+magnetics-1366028?r=sp</t>
+  </si>
+  <si>
+    <t>R8, R9, R10,R16</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1273,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,10 +1291,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -1360,10 +1360,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>32</v>
@@ -1372,10 +1372,10 @@
         <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1452,22 +1452,22 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1521,22 +1521,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1544,22 +1544,22 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1567,22 +1567,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1590,22 +1590,22 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1631,15 +1631,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -1648,10 +1648,10 @@
         <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1673,7 +1673,7 @@
       <c r="F17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1751,10 +1751,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
@@ -1763,10 +1763,10 @@
         <v>55</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1774,22 +1774,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1797,10 +1797,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1809,10 +1809,10 @@
         <v>18</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1823,7 +1823,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>49</v>
@@ -1832,10 +1832,10 @@
         <v>18</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1866,22 +1866,22 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1889,22 +1889,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1912,22 +1912,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1935,22 +1935,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1958,41 +1958,41 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2004,8 +2004,9 @@
     <hyperlink ref="G20" r:id="rId2"/>
     <hyperlink ref="G21" r:id="rId3"/>
     <hyperlink ref="G31" r:id="rId4"/>
+    <hyperlink ref="G17" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>